<commit_message>
Unknown power module BOM xlsx change.
</commit_message>
<xml_diff>
--- a/lta-power-module/fab runs/lta-power-module-v1_0-2022-05-16/Power module BOM v1_0.xlsx
+++ b/lta-power-module/fab runs/lta-power-module-v1_0-2022-05-16/Power module BOM v1_0.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\akimb\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\akimb\Documents\PCB CAD Projects\like-the-art\lta-power-module\fab runs\lta-power-module-v1_0-2022-05-16\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4D1A1F4-3137-470F-AAD9-4D0329FF80E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CAC191C-7BE1-420E-8E62-E8946E14B365}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2376" yWindow="2400" windowWidth="21600" windowHeight="12384" xr2:uid="{26CB0560-64BE-4098-B679-B872FE3FF68C}"/>
+    <workbookView xWindow="3720" yWindow="1524" windowWidth="22416" windowHeight="13368" xr2:uid="{26CB0560-64BE-4098-B679-B872FE3FF68C}"/>
   </bookViews>
   <sheets>
     <sheet name="PCB BOM" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,6 @@
     <sheet name="DigiKey-order-2022-05-10" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1125,10 +1124,10 @@
   <dimension ref="A1:J28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozenSplit"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="E16" sqref="E16"/>
+      <selection pane="bottomRight" activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1439,7 +1438,7 @@
       <c r="F10" t="s">
         <v>45</v>
       </c>
-      <c r="G10">
+      <c r="G10" s="5">
         <v>532530270</v>
       </c>
       <c r="H10" t="s">

</xml_diff>